<commit_message>
Update CPMMWithERC20Shares test file
</commit_message>
<xml_diff>
--- a/hackathon.xlsx
+++ b/hackathon.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="96">
   <si>
     <t>Casino</t>
   </si>
@@ -167,6 +168,138 @@
   </si>
   <si>
     <t>denom</t>
+  </si>
+  <si>
+    <t>🧠 Why use a CFMM in a prediction market?</t>
+  </si>
+  <si>
+    <t>1. Price = Implied Probability</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expect </t>
+  </si>
+  <si>
+    <t>mint</t>
+  </si>
+  <si>
+    <t>If 1 YES token pays $1 if the event happens, then its price reflects the market's belief.</t>
+  </si>
+  <si>
+    <t>pool</t>
+  </si>
+  <si>
+    <t>alice</t>
+  </si>
+  <si>
+    <t>$0.50 → 50% chance</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>Step 1</t>
+  </si>
+  <si>
+    <t>$0.90 → 90% chance</t>
+  </si>
+  <si>
+    <t>here</t>
+  </si>
+  <si>
+    <t>CFMM ensures prices move automatically with buying/selling pressure:</t>
+  </si>
+  <si>
+    <t>If someone buys lots of YES, price rises → implied probability goes up.</t>
+  </si>
+  <si>
+    <t>Step 2</t>
+  </si>
+  <si>
+    <t>If someone sells YES, price falls → belief goes down.</t>
+  </si>
+  <si>
+    <t>2. Liquidity without Counterparty</t>
+  </si>
+  <si>
+    <t>Traditional order books need buyers/sellers at each price.</t>
+  </si>
+  <si>
+    <t>Step 3</t>
+  </si>
+  <si>
+    <t>CFMM lets you trade anytime at a price determined by the curve.</t>
+  </si>
+  <si>
+    <t>E.g. Polymarket, Uniswap, and other AMM-based systems work this way.</t>
+  </si>
+  <si>
+    <t>Without CFMM, you'd need limit orders or market makers to manually adjust quotes.</t>
+  </si>
+  <si>
+    <t>3. Price Impact = Confidence Weight</t>
+  </si>
+  <si>
+    <t>The price impact is intentional:</t>
+  </si>
+  <si>
+    <t>Buying a large number of YES tokens pushes the price up.</t>
+  </si>
+  <si>
+    <t>This encodes how confident the buyer is in their belief.</t>
+  </si>
+  <si>
+    <t>Larger bets = more confident = more price movement.</t>
+  </si>
+  <si>
+    <t>This is why CFMMs are a natural fit: they reward early bettors with better prices and penalize late or large bettors unless they’re highly confident.</t>
+  </si>
+  <si>
+    <t>🧮 But Why Not Cap the Price at $1?</t>
+  </si>
+  <si>
+    <t>It is capped: a YES token can’t be worth more than $1 at resolution.</t>
+  </si>
+  <si>
+    <t>But the market price before resolution reflects the current odds and demand.</t>
+  </si>
+  <si>
+    <t>If someone is overpaying (e.g. paying $1.25 to win $1), it just means the curve pushed past their breakeven — and they lose if they're wrong.</t>
+  </si>
+  <si>
+    <t>🔄 Summary: Why CFMM?</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Why CFMM Helps</t>
+  </si>
+  <si>
+    <t>Belief Aggregation</t>
+  </si>
+  <si>
+    <t>Price moves encode crowd belief</t>
+  </si>
+  <si>
+    <t>Always-on Liquidity</t>
+  </si>
+  <si>
+    <t>No need for counterparties</t>
+  </si>
+  <si>
+    <t>Confidence-weighted Pricing</t>
+  </si>
+  <si>
+    <t>Bigger bets shift price more</t>
+  </si>
+  <si>
+    <t>Simplicity</t>
+  </si>
+  <si>
+    <t>Easy math, no order book needed</t>
   </si>
 </sst>
 </file>
@@ -176,7 +309,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -230,8 +363,21 @@
       <color rgb="FF9CDCFE"/>
       <name val="&quot;Droid Sans Mono&quot;"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -244,6 +390,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -251,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -301,6 +453,21 @@
     <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -310,6 +477,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1215,4 +1386,3368 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="E1" s="17"/>
+    </row>
+    <row r="2">
+      <c r="E2" s="17"/>
+      <c r="G2" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="E3" s="17"/>
+      <c r="G3" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="E4" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="6">
+        <v>500.0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>500.0</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="G5" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="6">
+        <v>500.0</v>
+      </c>
+      <c r="C6" s="6">
+        <v>500.0</v>
+      </c>
+      <c r="D6" s="11">
+        <f>B6*C6</f>
+        <v>250000</v>
+      </c>
+      <c r="E6" s="17">
+        <f>C6/sum(B6:C6)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="21"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="G7" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="11">
+        <f t="shared" ref="B8:C8" si="1">B7+B6</f>
+        <v>500</v>
+      </c>
+      <c r="C8" s="11">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="E8" s="17"/>
+      <c r="G8" s="21"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="17"/>
+      <c r="G9" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="6">
+        <v>100.0</v>
+      </c>
+      <c r="C10" s="6">
+        <v>100.0</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="G10" s="21"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="11">
+        <f>D6/C11</f>
+        <v>416.6666667</v>
+      </c>
+      <c r="C11" s="11">
+        <f>C10+C6</f>
+        <v>600</v>
+      </c>
+      <c r="D11" s="11">
+        <f>B11*C11</f>
+        <v>250000</v>
+      </c>
+      <c r="E11" s="17">
+        <f>C11/sum(B11:C11)</f>
+        <v>0.5901639344</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="11">
+        <f t="shared" ref="B12:C12" si="2">B6-B11+B7+B10</f>
+        <v>183.3333333</v>
+      </c>
+      <c r="C12" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="17"/>
+      <c r="F12" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="11">
+        <f t="shared" ref="B13:C13" si="3">B11+B12</f>
+        <v>600</v>
+      </c>
+      <c r="C13" s="11">
+        <f t="shared" si="3"/>
+        <v>600</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="G13" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="G14" s="21"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="6">
+        <v>100.0</v>
+      </c>
+      <c r="C15" s="6">
+        <v>100.0</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="G15" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="11">
+        <f>D11/C16</f>
+        <v>357.1428571</v>
+      </c>
+      <c r="C16" s="11">
+        <f>C15+C11</f>
+        <v>700</v>
+      </c>
+      <c r="D16" s="11">
+        <f>B16*C16</f>
+        <v>250000</v>
+      </c>
+      <c r="E16" s="17">
+        <f>C16/sum(B16:C16)</f>
+        <v>0.6621621622</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="11">
+        <f t="shared" ref="B17:C17" si="4">B11-B16+B12+B15</f>
+        <v>342.8571429</v>
+      </c>
+      <c r="C17" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="17">
+        <f>B17-B12</f>
+        <v>159.5238095</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="21"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="11">
+        <f t="shared" ref="B18:C18" si="5">B16+B17</f>
+        <v>700</v>
+      </c>
+      <c r="C18" s="11">
+        <f t="shared" si="5"/>
+        <v>700</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="G18" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="G19" s="21"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="E20" s="17"/>
+      <c r="G20" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="11">
+        <f>D16/C21</f>
+        <v>356.6333809</v>
+      </c>
+      <c r="C21" s="11">
+        <f>C20+C16</f>
+        <v>701</v>
+      </c>
+      <c r="D21" s="11">
+        <f>B21*C21</f>
+        <v>250000</v>
+      </c>
+      <c r="E21" s="17">
+        <f>C21/sum(B21:C21)</f>
+        <v>0.6628005627</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="21"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="11">
+        <f t="shared" ref="B22:C22" si="6">B16-B21+B17+B20</f>
+        <v>344.3666191</v>
+      </c>
+      <c r="C22" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="17"/>
+      <c r="F22" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="11">
+        <f t="shared" ref="B23:C23" si="7">B21+B22</f>
+        <v>701</v>
+      </c>
+      <c r="C23" s="11">
+        <f t="shared" si="7"/>
+        <v>701</v>
+      </c>
+      <c r="E23" s="17"/>
+      <c r="G23" s="21"/>
+    </row>
+    <row r="24">
+      <c r="E24" s="17"/>
+      <c r="G24" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="E25" s="17"/>
+      <c r="G25" s="21"/>
+    </row>
+    <row r="26">
+      <c r="E26" s="17"/>
+      <c r="G26" s="19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="E27" s="17"/>
+      <c r="G27" s="21"/>
+    </row>
+    <row r="28">
+      <c r="E28" s="17"/>
+      <c r="G28" s="19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="E29" s="17"/>
+      <c r="G29" s="21"/>
+    </row>
+    <row r="30">
+      <c r="E30" s="17"/>
+      <c r="G30" s="19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="E31" s="17"/>
+      <c r="G31" s="21"/>
+    </row>
+    <row r="32">
+      <c r="E32" s="17"/>
+      <c r="G32" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="E33" s="17"/>
+      <c r="G33" s="21"/>
+    </row>
+    <row r="34">
+      <c r="E34" s="17"/>
+      <c r="G34" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="E35" s="17"/>
+      <c r="G35" s="21"/>
+    </row>
+    <row r="36">
+      <c r="E36" s="17"/>
+      <c r="G36" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="E37" s="17"/>
+      <c r="G37" s="21"/>
+    </row>
+    <row r="38">
+      <c r="E38" s="17"/>
+      <c r="G38" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="E39" s="17"/>
+      <c r="G39" s="22"/>
+    </row>
+    <row r="40">
+      <c r="E40" s="17"/>
+      <c r="G40" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="E41" s="17"/>
+      <c r="G41" s="22"/>
+    </row>
+    <row r="42">
+      <c r="E42" s="17"/>
+      <c r="G42" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="E43" s="17"/>
+      <c r="G43" s="22"/>
+    </row>
+    <row r="44">
+      <c r="E44" s="17"/>
+      <c r="G44" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="E45" s="17"/>
+      <c r="G45" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="E46" s="17"/>
+      <c r="G46" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="H46" s="23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="E47" s="17"/>
+      <c r="G47" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="H47" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="E48" s="17"/>
+      <c r="G48" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="H48" s="18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="E49" s="17"/>
+      <c r="G49" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="H49" s="18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="E50" s="17"/>
+      <c r="G50" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="H50" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="E51" s="17"/>
+    </row>
+    <row r="52">
+      <c r="E52" s="17"/>
+    </row>
+    <row r="53">
+      <c r="E53" s="17"/>
+    </row>
+    <row r="54">
+      <c r="E54" s="17"/>
+    </row>
+    <row r="55">
+      <c r="E55" s="17"/>
+    </row>
+    <row r="56">
+      <c r="E56" s="17"/>
+    </row>
+    <row r="57">
+      <c r="E57" s="17"/>
+    </row>
+    <row r="58">
+      <c r="E58" s="17"/>
+    </row>
+    <row r="59">
+      <c r="E59" s="17"/>
+    </row>
+    <row r="60">
+      <c r="E60" s="17"/>
+    </row>
+    <row r="61">
+      <c r="E61" s="17"/>
+    </row>
+    <row r="62">
+      <c r="E62" s="17"/>
+    </row>
+    <row r="63">
+      <c r="E63" s="17"/>
+    </row>
+    <row r="64">
+      <c r="E64" s="17"/>
+    </row>
+    <row r="65">
+      <c r="E65" s="17"/>
+    </row>
+    <row r="66">
+      <c r="E66" s="17"/>
+    </row>
+    <row r="67">
+      <c r="E67" s="17"/>
+    </row>
+    <row r="68">
+      <c r="E68" s="17"/>
+    </row>
+    <row r="69">
+      <c r="E69" s="17"/>
+    </row>
+    <row r="70">
+      <c r="E70" s="17"/>
+    </row>
+    <row r="71">
+      <c r="E71" s="17"/>
+    </row>
+    <row r="72">
+      <c r="E72" s="17"/>
+    </row>
+    <row r="73">
+      <c r="E73" s="17"/>
+    </row>
+    <row r="74">
+      <c r="E74" s="17"/>
+    </row>
+    <row r="75">
+      <c r="E75" s="17"/>
+    </row>
+    <row r="76">
+      <c r="E76" s="17"/>
+    </row>
+    <row r="77">
+      <c r="E77" s="17"/>
+    </row>
+    <row r="78">
+      <c r="E78" s="17"/>
+    </row>
+    <row r="79">
+      <c r="E79" s="17"/>
+    </row>
+    <row r="80">
+      <c r="E80" s="17"/>
+    </row>
+    <row r="81">
+      <c r="E81" s="17"/>
+    </row>
+    <row r="82">
+      <c r="E82" s="17"/>
+    </row>
+    <row r="83">
+      <c r="E83" s="17"/>
+    </row>
+    <row r="84">
+      <c r="E84" s="17"/>
+    </row>
+    <row r="85">
+      <c r="E85" s="17"/>
+    </row>
+    <row r="86">
+      <c r="E86" s="17"/>
+    </row>
+    <row r="87">
+      <c r="E87" s="17"/>
+    </row>
+    <row r="88">
+      <c r="E88" s="17"/>
+    </row>
+    <row r="89">
+      <c r="E89" s="17"/>
+    </row>
+    <row r="90">
+      <c r="E90" s="17"/>
+    </row>
+    <row r="91">
+      <c r="E91" s="17"/>
+    </row>
+    <row r="92">
+      <c r="E92" s="17"/>
+    </row>
+    <row r="93">
+      <c r="E93" s="17"/>
+    </row>
+    <row r="94">
+      <c r="E94" s="17"/>
+    </row>
+    <row r="95">
+      <c r="E95" s="17"/>
+    </row>
+    <row r="96">
+      <c r="E96" s="17"/>
+    </row>
+    <row r="97">
+      <c r="E97" s="17"/>
+    </row>
+    <row r="98">
+      <c r="E98" s="17"/>
+    </row>
+    <row r="99">
+      <c r="E99" s="17"/>
+    </row>
+    <row r="100">
+      <c r="E100" s="17"/>
+    </row>
+    <row r="101">
+      <c r="E101" s="17"/>
+    </row>
+    <row r="102">
+      <c r="E102" s="17"/>
+    </row>
+    <row r="103">
+      <c r="E103" s="17"/>
+    </row>
+    <row r="104">
+      <c r="E104" s="17"/>
+    </row>
+    <row r="105">
+      <c r="E105" s="17"/>
+    </row>
+    <row r="106">
+      <c r="E106" s="17"/>
+    </row>
+    <row r="107">
+      <c r="E107" s="17"/>
+    </row>
+    <row r="108">
+      <c r="E108" s="17"/>
+    </row>
+    <row r="109">
+      <c r="E109" s="17"/>
+    </row>
+    <row r="110">
+      <c r="E110" s="17"/>
+    </row>
+    <row r="111">
+      <c r="E111" s="17"/>
+    </row>
+    <row r="112">
+      <c r="E112" s="17"/>
+    </row>
+    <row r="113">
+      <c r="E113" s="17"/>
+    </row>
+    <row r="114">
+      <c r="E114" s="17"/>
+    </row>
+    <row r="115">
+      <c r="E115" s="17"/>
+    </row>
+    <row r="116">
+      <c r="E116" s="17"/>
+    </row>
+    <row r="117">
+      <c r="E117" s="17"/>
+    </row>
+    <row r="118">
+      <c r="E118" s="17"/>
+    </row>
+    <row r="119">
+      <c r="E119" s="17"/>
+    </row>
+    <row r="120">
+      <c r="E120" s="17"/>
+    </row>
+    <row r="121">
+      <c r="E121" s="17"/>
+    </row>
+    <row r="122">
+      <c r="E122" s="17"/>
+    </row>
+    <row r="123">
+      <c r="E123" s="17"/>
+    </row>
+    <row r="124">
+      <c r="E124" s="17"/>
+    </row>
+    <row r="125">
+      <c r="E125" s="17"/>
+    </row>
+    <row r="126">
+      <c r="E126" s="17"/>
+    </row>
+    <row r="127">
+      <c r="E127" s="17"/>
+    </row>
+    <row r="128">
+      <c r="E128" s="17"/>
+    </row>
+    <row r="129">
+      <c r="E129" s="17"/>
+    </row>
+    <row r="130">
+      <c r="E130" s="17"/>
+    </row>
+    <row r="131">
+      <c r="E131" s="17"/>
+    </row>
+    <row r="132">
+      <c r="E132" s="17"/>
+    </row>
+    <row r="133">
+      <c r="E133" s="17"/>
+    </row>
+    <row r="134">
+      <c r="E134" s="17"/>
+    </row>
+    <row r="135">
+      <c r="E135" s="17"/>
+    </row>
+    <row r="136">
+      <c r="E136" s="17"/>
+    </row>
+    <row r="137">
+      <c r="E137" s="17"/>
+    </row>
+    <row r="138">
+      <c r="E138" s="17"/>
+    </row>
+    <row r="139">
+      <c r="E139" s="17"/>
+    </row>
+    <row r="140">
+      <c r="E140" s="17"/>
+    </row>
+    <row r="141">
+      <c r="E141" s="17"/>
+    </row>
+    <row r="142">
+      <c r="E142" s="17"/>
+    </row>
+    <row r="143">
+      <c r="E143" s="17"/>
+    </row>
+    <row r="144">
+      <c r="E144" s="17"/>
+    </row>
+    <row r="145">
+      <c r="E145" s="17"/>
+    </row>
+    <row r="146">
+      <c r="E146" s="17"/>
+    </row>
+    <row r="147">
+      <c r="E147" s="17"/>
+    </row>
+    <row r="148">
+      <c r="E148" s="17"/>
+    </row>
+    <row r="149">
+      <c r="E149" s="17"/>
+    </row>
+    <row r="150">
+      <c r="E150" s="17"/>
+    </row>
+    <row r="151">
+      <c r="E151" s="17"/>
+    </row>
+    <row r="152">
+      <c r="E152" s="17"/>
+    </row>
+    <row r="153">
+      <c r="E153" s="17"/>
+    </row>
+    <row r="154">
+      <c r="E154" s="17"/>
+    </row>
+    <row r="155">
+      <c r="E155" s="17"/>
+    </row>
+    <row r="156">
+      <c r="E156" s="17"/>
+    </row>
+    <row r="157">
+      <c r="E157" s="17"/>
+    </row>
+    <row r="158">
+      <c r="E158" s="17"/>
+    </row>
+    <row r="159">
+      <c r="E159" s="17"/>
+    </row>
+    <row r="160">
+      <c r="E160" s="17"/>
+    </row>
+    <row r="161">
+      <c r="E161" s="17"/>
+    </row>
+    <row r="162">
+      <c r="E162" s="17"/>
+    </row>
+    <row r="163">
+      <c r="E163" s="17"/>
+    </row>
+    <row r="164">
+      <c r="E164" s="17"/>
+    </row>
+    <row r="165">
+      <c r="E165" s="17"/>
+    </row>
+    <row r="166">
+      <c r="E166" s="17"/>
+    </row>
+    <row r="167">
+      <c r="E167" s="17"/>
+    </row>
+    <row r="168">
+      <c r="E168" s="17"/>
+    </row>
+    <row r="169">
+      <c r="E169" s="17"/>
+    </row>
+    <row r="170">
+      <c r="E170" s="17"/>
+    </row>
+    <row r="171">
+      <c r="E171" s="17"/>
+    </row>
+    <row r="172">
+      <c r="E172" s="17"/>
+    </row>
+    <row r="173">
+      <c r="E173" s="17"/>
+    </row>
+    <row r="174">
+      <c r="E174" s="17"/>
+    </row>
+    <row r="175">
+      <c r="E175" s="17"/>
+    </row>
+    <row r="176">
+      <c r="E176" s="17"/>
+    </row>
+    <row r="177">
+      <c r="E177" s="17"/>
+    </row>
+    <row r="178">
+      <c r="E178" s="17"/>
+    </row>
+    <row r="179">
+      <c r="E179" s="17"/>
+    </row>
+    <row r="180">
+      <c r="E180" s="17"/>
+    </row>
+    <row r="181">
+      <c r="E181" s="17"/>
+    </row>
+    <row r="182">
+      <c r="E182" s="17"/>
+    </row>
+    <row r="183">
+      <c r="E183" s="17"/>
+    </row>
+    <row r="184">
+      <c r="E184" s="17"/>
+    </row>
+    <row r="185">
+      <c r="E185" s="17"/>
+    </row>
+    <row r="186">
+      <c r="E186" s="17"/>
+    </row>
+    <row r="187">
+      <c r="E187" s="17"/>
+    </row>
+    <row r="188">
+      <c r="E188" s="17"/>
+    </row>
+    <row r="189">
+      <c r="E189" s="17"/>
+    </row>
+    <row r="190">
+      <c r="E190" s="17"/>
+    </row>
+    <row r="191">
+      <c r="E191" s="17"/>
+    </row>
+    <row r="192">
+      <c r="E192" s="17"/>
+    </row>
+    <row r="193">
+      <c r="E193" s="17"/>
+    </row>
+    <row r="194">
+      <c r="E194" s="17"/>
+    </row>
+    <row r="195">
+      <c r="E195" s="17"/>
+    </row>
+    <row r="196">
+      <c r="E196" s="17"/>
+    </row>
+    <row r="197">
+      <c r="E197" s="17"/>
+    </row>
+    <row r="198">
+      <c r="E198" s="17"/>
+    </row>
+    <row r="199">
+      <c r="E199" s="17"/>
+    </row>
+    <row r="200">
+      <c r="E200" s="17"/>
+    </row>
+    <row r="201">
+      <c r="E201" s="17"/>
+    </row>
+    <row r="202">
+      <c r="E202" s="17"/>
+    </row>
+    <row r="203">
+      <c r="E203" s="17"/>
+    </row>
+    <row r="204">
+      <c r="E204" s="17"/>
+    </row>
+    <row r="205">
+      <c r="E205" s="17"/>
+    </row>
+    <row r="206">
+      <c r="E206" s="17"/>
+    </row>
+    <row r="207">
+      <c r="E207" s="17"/>
+    </row>
+    <row r="208">
+      <c r="E208" s="17"/>
+    </row>
+    <row r="209">
+      <c r="E209" s="17"/>
+    </row>
+    <row r="210">
+      <c r="E210" s="17"/>
+    </row>
+    <row r="211">
+      <c r="E211" s="17"/>
+    </row>
+    <row r="212">
+      <c r="E212" s="17"/>
+    </row>
+    <row r="213">
+      <c r="E213" s="17"/>
+    </row>
+    <row r="214">
+      <c r="E214" s="17"/>
+    </row>
+    <row r="215">
+      <c r="E215" s="17"/>
+    </row>
+    <row r="216">
+      <c r="E216" s="17"/>
+    </row>
+    <row r="217">
+      <c r="E217" s="17"/>
+    </row>
+    <row r="218">
+      <c r="E218" s="17"/>
+    </row>
+    <row r="219">
+      <c r="E219" s="17"/>
+    </row>
+    <row r="220">
+      <c r="E220" s="17"/>
+    </row>
+    <row r="221">
+      <c r="E221" s="17"/>
+    </row>
+    <row r="222">
+      <c r="E222" s="17"/>
+    </row>
+    <row r="223">
+      <c r="E223" s="17"/>
+    </row>
+    <row r="224">
+      <c r="E224" s="17"/>
+    </row>
+    <row r="225">
+      <c r="E225" s="17"/>
+    </row>
+    <row r="226">
+      <c r="E226" s="17"/>
+    </row>
+    <row r="227">
+      <c r="E227" s="17"/>
+    </row>
+    <row r="228">
+      <c r="E228" s="17"/>
+    </row>
+    <row r="229">
+      <c r="E229" s="17"/>
+    </row>
+    <row r="230">
+      <c r="E230" s="17"/>
+    </row>
+    <row r="231">
+      <c r="E231" s="17"/>
+    </row>
+    <row r="232">
+      <c r="E232" s="17"/>
+    </row>
+    <row r="233">
+      <c r="E233" s="17"/>
+    </row>
+    <row r="234">
+      <c r="E234" s="17"/>
+    </row>
+    <row r="235">
+      <c r="E235" s="17"/>
+    </row>
+    <row r="236">
+      <c r="E236" s="17"/>
+    </row>
+    <row r="237">
+      <c r="E237" s="17"/>
+    </row>
+    <row r="238">
+      <c r="E238" s="17"/>
+    </row>
+    <row r="239">
+      <c r="E239" s="17"/>
+    </row>
+    <row r="240">
+      <c r="E240" s="17"/>
+    </row>
+    <row r="241">
+      <c r="E241" s="17"/>
+    </row>
+    <row r="242">
+      <c r="E242" s="17"/>
+    </row>
+    <row r="243">
+      <c r="E243" s="17"/>
+    </row>
+    <row r="244">
+      <c r="E244" s="17"/>
+    </row>
+    <row r="245">
+      <c r="E245" s="17"/>
+    </row>
+    <row r="246">
+      <c r="E246" s="17"/>
+    </row>
+    <row r="247">
+      <c r="E247" s="17"/>
+    </row>
+    <row r="248">
+      <c r="E248" s="17"/>
+    </row>
+    <row r="249">
+      <c r="E249" s="17"/>
+    </row>
+    <row r="250">
+      <c r="E250" s="17"/>
+    </row>
+    <row r="251">
+      <c r="E251" s="17"/>
+    </row>
+    <row r="252">
+      <c r="E252" s="17"/>
+    </row>
+    <row r="253">
+      <c r="E253" s="17"/>
+    </row>
+    <row r="254">
+      <c r="E254" s="17"/>
+    </row>
+    <row r="255">
+      <c r="E255" s="17"/>
+    </row>
+    <row r="256">
+      <c r="E256" s="17"/>
+    </row>
+    <row r="257">
+      <c r="E257" s="17"/>
+    </row>
+    <row r="258">
+      <c r="E258" s="17"/>
+    </row>
+    <row r="259">
+      <c r="E259" s="17"/>
+    </row>
+    <row r="260">
+      <c r="E260" s="17"/>
+    </row>
+    <row r="261">
+      <c r="E261" s="17"/>
+    </row>
+    <row r="262">
+      <c r="E262" s="17"/>
+    </row>
+    <row r="263">
+      <c r="E263" s="17"/>
+    </row>
+    <row r="264">
+      <c r="E264" s="17"/>
+    </row>
+    <row r="265">
+      <c r="E265" s="17"/>
+    </row>
+    <row r="266">
+      <c r="E266" s="17"/>
+    </row>
+    <row r="267">
+      <c r="E267" s="17"/>
+    </row>
+    <row r="268">
+      <c r="E268" s="17"/>
+    </row>
+    <row r="269">
+      <c r="E269" s="17"/>
+    </row>
+    <row r="270">
+      <c r="E270" s="17"/>
+    </row>
+    <row r="271">
+      <c r="E271" s="17"/>
+    </row>
+    <row r="272">
+      <c r="E272" s="17"/>
+    </row>
+    <row r="273">
+      <c r="E273" s="17"/>
+    </row>
+    <row r="274">
+      <c r="E274" s="17"/>
+    </row>
+    <row r="275">
+      <c r="E275" s="17"/>
+    </row>
+    <row r="276">
+      <c r="E276" s="17"/>
+    </row>
+    <row r="277">
+      <c r="E277" s="17"/>
+    </row>
+    <row r="278">
+      <c r="E278" s="17"/>
+    </row>
+    <row r="279">
+      <c r="E279" s="17"/>
+    </row>
+    <row r="280">
+      <c r="E280" s="17"/>
+    </row>
+    <row r="281">
+      <c r="E281" s="17"/>
+    </row>
+    <row r="282">
+      <c r="E282" s="17"/>
+    </row>
+    <row r="283">
+      <c r="E283" s="17"/>
+    </row>
+    <row r="284">
+      <c r="E284" s="17"/>
+    </row>
+    <row r="285">
+      <c r="E285" s="17"/>
+    </row>
+    <row r="286">
+      <c r="E286" s="17"/>
+    </row>
+    <row r="287">
+      <c r="E287" s="17"/>
+    </row>
+    <row r="288">
+      <c r="E288" s="17"/>
+    </row>
+    <row r="289">
+      <c r="E289" s="17"/>
+    </row>
+    <row r="290">
+      <c r="E290" s="17"/>
+    </row>
+    <row r="291">
+      <c r="E291" s="17"/>
+    </row>
+    <row r="292">
+      <c r="E292" s="17"/>
+    </row>
+    <row r="293">
+      <c r="E293" s="17"/>
+    </row>
+    <row r="294">
+      <c r="E294" s="17"/>
+    </row>
+    <row r="295">
+      <c r="E295" s="17"/>
+    </row>
+    <row r="296">
+      <c r="E296" s="17"/>
+    </row>
+    <row r="297">
+      <c r="E297" s="17"/>
+    </row>
+    <row r="298">
+      <c r="E298" s="17"/>
+    </row>
+    <row r="299">
+      <c r="E299" s="17"/>
+    </row>
+    <row r="300">
+      <c r="E300" s="17"/>
+    </row>
+    <row r="301">
+      <c r="E301" s="17"/>
+    </row>
+    <row r="302">
+      <c r="E302" s="17"/>
+    </row>
+    <row r="303">
+      <c r="E303" s="17"/>
+    </row>
+    <row r="304">
+      <c r="E304" s="17"/>
+    </row>
+    <row r="305">
+      <c r="E305" s="17"/>
+    </row>
+    <row r="306">
+      <c r="E306" s="17"/>
+    </row>
+    <row r="307">
+      <c r="E307" s="17"/>
+    </row>
+    <row r="308">
+      <c r="E308" s="17"/>
+    </row>
+    <row r="309">
+      <c r="E309" s="17"/>
+    </row>
+    <row r="310">
+      <c r="E310" s="17"/>
+    </row>
+    <row r="311">
+      <c r="E311" s="17"/>
+    </row>
+    <row r="312">
+      <c r="E312" s="17"/>
+    </row>
+    <row r="313">
+      <c r="E313" s="17"/>
+    </row>
+    <row r="314">
+      <c r="E314" s="17"/>
+    </row>
+    <row r="315">
+      <c r="E315" s="17"/>
+    </row>
+    <row r="316">
+      <c r="E316" s="17"/>
+    </row>
+    <row r="317">
+      <c r="E317" s="17"/>
+    </row>
+    <row r="318">
+      <c r="E318" s="17"/>
+    </row>
+    <row r="319">
+      <c r="E319" s="17"/>
+    </row>
+    <row r="320">
+      <c r="E320" s="17"/>
+    </row>
+    <row r="321">
+      <c r="E321" s="17"/>
+    </row>
+    <row r="322">
+      <c r="E322" s="17"/>
+    </row>
+    <row r="323">
+      <c r="E323" s="17"/>
+    </row>
+    <row r="324">
+      <c r="E324" s="17"/>
+    </row>
+    <row r="325">
+      <c r="E325" s="17"/>
+    </row>
+    <row r="326">
+      <c r="E326" s="17"/>
+    </row>
+    <row r="327">
+      <c r="E327" s="17"/>
+    </row>
+    <row r="328">
+      <c r="E328" s="17"/>
+    </row>
+    <row r="329">
+      <c r="E329" s="17"/>
+    </row>
+    <row r="330">
+      <c r="E330" s="17"/>
+    </row>
+    <row r="331">
+      <c r="E331" s="17"/>
+    </row>
+    <row r="332">
+      <c r="E332" s="17"/>
+    </row>
+    <row r="333">
+      <c r="E333" s="17"/>
+    </row>
+    <row r="334">
+      <c r="E334" s="17"/>
+    </row>
+    <row r="335">
+      <c r="E335" s="17"/>
+    </row>
+    <row r="336">
+      <c r="E336" s="17"/>
+    </row>
+    <row r="337">
+      <c r="E337" s="17"/>
+    </row>
+    <row r="338">
+      <c r="E338" s="17"/>
+    </row>
+    <row r="339">
+      <c r="E339" s="17"/>
+    </row>
+    <row r="340">
+      <c r="E340" s="17"/>
+    </row>
+    <row r="341">
+      <c r="E341" s="17"/>
+    </row>
+    <row r="342">
+      <c r="E342" s="17"/>
+    </row>
+    <row r="343">
+      <c r="E343" s="17"/>
+    </row>
+    <row r="344">
+      <c r="E344" s="17"/>
+    </row>
+    <row r="345">
+      <c r="E345" s="17"/>
+    </row>
+    <row r="346">
+      <c r="E346" s="17"/>
+    </row>
+    <row r="347">
+      <c r="E347" s="17"/>
+    </row>
+    <row r="348">
+      <c r="E348" s="17"/>
+    </row>
+    <row r="349">
+      <c r="E349" s="17"/>
+    </row>
+    <row r="350">
+      <c r="E350" s="17"/>
+    </row>
+    <row r="351">
+      <c r="E351" s="17"/>
+    </row>
+    <row r="352">
+      <c r="E352" s="17"/>
+    </row>
+    <row r="353">
+      <c r="E353" s="17"/>
+    </row>
+    <row r="354">
+      <c r="E354" s="17"/>
+    </row>
+    <row r="355">
+      <c r="E355" s="17"/>
+    </row>
+    <row r="356">
+      <c r="E356" s="17"/>
+    </row>
+    <row r="357">
+      <c r="E357" s="17"/>
+    </row>
+    <row r="358">
+      <c r="E358" s="17"/>
+    </row>
+    <row r="359">
+      <c r="E359" s="17"/>
+    </row>
+    <row r="360">
+      <c r="E360" s="17"/>
+    </row>
+    <row r="361">
+      <c r="E361" s="17"/>
+    </row>
+    <row r="362">
+      <c r="E362" s="17"/>
+    </row>
+    <row r="363">
+      <c r="E363" s="17"/>
+    </row>
+    <row r="364">
+      <c r="E364" s="17"/>
+    </row>
+    <row r="365">
+      <c r="E365" s="17"/>
+    </row>
+    <row r="366">
+      <c r="E366" s="17"/>
+    </row>
+    <row r="367">
+      <c r="E367" s="17"/>
+    </row>
+    <row r="368">
+      <c r="E368" s="17"/>
+    </row>
+    <row r="369">
+      <c r="E369" s="17"/>
+    </row>
+    <row r="370">
+      <c r="E370" s="17"/>
+    </row>
+    <row r="371">
+      <c r="E371" s="17"/>
+    </row>
+    <row r="372">
+      <c r="E372" s="17"/>
+    </row>
+    <row r="373">
+      <c r="E373" s="17"/>
+    </row>
+    <row r="374">
+      <c r="E374" s="17"/>
+    </row>
+    <row r="375">
+      <c r="E375" s="17"/>
+    </row>
+    <row r="376">
+      <c r="E376" s="17"/>
+    </row>
+    <row r="377">
+      <c r="E377" s="17"/>
+    </row>
+    <row r="378">
+      <c r="E378" s="17"/>
+    </row>
+    <row r="379">
+      <c r="E379" s="17"/>
+    </row>
+    <row r="380">
+      <c r="E380" s="17"/>
+    </row>
+    <row r="381">
+      <c r="E381" s="17"/>
+    </row>
+    <row r="382">
+      <c r="E382" s="17"/>
+    </row>
+    <row r="383">
+      <c r="E383" s="17"/>
+    </row>
+    <row r="384">
+      <c r="E384" s="17"/>
+    </row>
+    <row r="385">
+      <c r="E385" s="17"/>
+    </row>
+    <row r="386">
+      <c r="E386" s="17"/>
+    </row>
+    <row r="387">
+      <c r="E387" s="17"/>
+    </row>
+    <row r="388">
+      <c r="E388" s="17"/>
+    </row>
+    <row r="389">
+      <c r="E389" s="17"/>
+    </row>
+    <row r="390">
+      <c r="E390" s="17"/>
+    </row>
+    <row r="391">
+      <c r="E391" s="17"/>
+    </row>
+    <row r="392">
+      <c r="E392" s="17"/>
+    </row>
+    <row r="393">
+      <c r="E393" s="17"/>
+    </row>
+    <row r="394">
+      <c r="E394" s="17"/>
+    </row>
+    <row r="395">
+      <c r="E395" s="17"/>
+    </row>
+    <row r="396">
+      <c r="E396" s="17"/>
+    </row>
+    <row r="397">
+      <c r="E397" s="17"/>
+    </row>
+    <row r="398">
+      <c r="E398" s="17"/>
+    </row>
+    <row r="399">
+      <c r="E399" s="17"/>
+    </row>
+    <row r="400">
+      <c r="E400" s="17"/>
+    </row>
+    <row r="401">
+      <c r="E401" s="17"/>
+    </row>
+    <row r="402">
+      <c r="E402" s="17"/>
+    </row>
+    <row r="403">
+      <c r="E403" s="17"/>
+    </row>
+    <row r="404">
+      <c r="E404" s="17"/>
+    </row>
+    <row r="405">
+      <c r="E405" s="17"/>
+    </row>
+    <row r="406">
+      <c r="E406" s="17"/>
+    </row>
+    <row r="407">
+      <c r="E407" s="17"/>
+    </row>
+    <row r="408">
+      <c r="E408" s="17"/>
+    </row>
+    <row r="409">
+      <c r="E409" s="17"/>
+    </row>
+    <row r="410">
+      <c r="E410" s="17"/>
+    </row>
+    <row r="411">
+      <c r="E411" s="17"/>
+    </row>
+    <row r="412">
+      <c r="E412" s="17"/>
+    </row>
+    <row r="413">
+      <c r="E413" s="17"/>
+    </row>
+    <row r="414">
+      <c r="E414" s="17"/>
+    </row>
+    <row r="415">
+      <c r="E415" s="17"/>
+    </row>
+    <row r="416">
+      <c r="E416" s="17"/>
+    </row>
+    <row r="417">
+      <c r="E417" s="17"/>
+    </row>
+    <row r="418">
+      <c r="E418" s="17"/>
+    </row>
+    <row r="419">
+      <c r="E419" s="17"/>
+    </row>
+    <row r="420">
+      <c r="E420" s="17"/>
+    </row>
+    <row r="421">
+      <c r="E421" s="17"/>
+    </row>
+    <row r="422">
+      <c r="E422" s="17"/>
+    </row>
+    <row r="423">
+      <c r="E423" s="17"/>
+    </row>
+    <row r="424">
+      <c r="E424" s="17"/>
+    </row>
+    <row r="425">
+      <c r="E425" s="17"/>
+    </row>
+    <row r="426">
+      <c r="E426" s="17"/>
+    </row>
+    <row r="427">
+      <c r="E427" s="17"/>
+    </row>
+    <row r="428">
+      <c r="E428" s="17"/>
+    </row>
+    <row r="429">
+      <c r="E429" s="17"/>
+    </row>
+    <row r="430">
+      <c r="E430" s="17"/>
+    </row>
+    <row r="431">
+      <c r="E431" s="17"/>
+    </row>
+    <row r="432">
+      <c r="E432" s="17"/>
+    </row>
+    <row r="433">
+      <c r="E433" s="17"/>
+    </row>
+    <row r="434">
+      <c r="E434" s="17"/>
+    </row>
+    <row r="435">
+      <c r="E435" s="17"/>
+    </row>
+    <row r="436">
+      <c r="E436" s="17"/>
+    </row>
+    <row r="437">
+      <c r="E437" s="17"/>
+    </row>
+    <row r="438">
+      <c r="E438" s="17"/>
+    </row>
+    <row r="439">
+      <c r="E439" s="17"/>
+    </row>
+    <row r="440">
+      <c r="E440" s="17"/>
+    </row>
+    <row r="441">
+      <c r="E441" s="17"/>
+    </row>
+    <row r="442">
+      <c r="E442" s="17"/>
+    </row>
+    <row r="443">
+      <c r="E443" s="17"/>
+    </row>
+    <row r="444">
+      <c r="E444" s="17"/>
+    </row>
+    <row r="445">
+      <c r="E445" s="17"/>
+    </row>
+    <row r="446">
+      <c r="E446" s="17"/>
+    </row>
+    <row r="447">
+      <c r="E447" s="17"/>
+    </row>
+    <row r="448">
+      <c r="E448" s="17"/>
+    </row>
+    <row r="449">
+      <c r="E449" s="17"/>
+    </row>
+    <row r="450">
+      <c r="E450" s="17"/>
+    </row>
+    <row r="451">
+      <c r="E451" s="17"/>
+    </row>
+    <row r="452">
+      <c r="E452" s="17"/>
+    </row>
+    <row r="453">
+      <c r="E453" s="17"/>
+    </row>
+    <row r="454">
+      <c r="E454" s="17"/>
+    </row>
+    <row r="455">
+      <c r="E455" s="17"/>
+    </row>
+    <row r="456">
+      <c r="E456" s="17"/>
+    </row>
+    <row r="457">
+      <c r="E457" s="17"/>
+    </row>
+    <row r="458">
+      <c r="E458" s="17"/>
+    </row>
+    <row r="459">
+      <c r="E459" s="17"/>
+    </row>
+    <row r="460">
+      <c r="E460" s="17"/>
+    </row>
+    <row r="461">
+      <c r="E461" s="17"/>
+    </row>
+    <row r="462">
+      <c r="E462" s="17"/>
+    </row>
+    <row r="463">
+      <c r="E463" s="17"/>
+    </row>
+    <row r="464">
+      <c r="E464" s="17"/>
+    </row>
+    <row r="465">
+      <c r="E465" s="17"/>
+    </row>
+    <row r="466">
+      <c r="E466" s="17"/>
+    </row>
+    <row r="467">
+      <c r="E467" s="17"/>
+    </row>
+    <row r="468">
+      <c r="E468" s="17"/>
+    </row>
+    <row r="469">
+      <c r="E469" s="17"/>
+    </row>
+    <row r="470">
+      <c r="E470" s="17"/>
+    </row>
+    <row r="471">
+      <c r="E471" s="17"/>
+    </row>
+    <row r="472">
+      <c r="E472" s="17"/>
+    </row>
+    <row r="473">
+      <c r="E473" s="17"/>
+    </row>
+    <row r="474">
+      <c r="E474" s="17"/>
+    </row>
+    <row r="475">
+      <c r="E475" s="17"/>
+    </row>
+    <row r="476">
+      <c r="E476" s="17"/>
+    </row>
+    <row r="477">
+      <c r="E477" s="17"/>
+    </row>
+    <row r="478">
+      <c r="E478" s="17"/>
+    </row>
+    <row r="479">
+      <c r="E479" s="17"/>
+    </row>
+    <row r="480">
+      <c r="E480" s="17"/>
+    </row>
+    <row r="481">
+      <c r="E481" s="17"/>
+    </row>
+    <row r="482">
+      <c r="E482" s="17"/>
+    </row>
+    <row r="483">
+      <c r="E483" s="17"/>
+    </row>
+    <row r="484">
+      <c r="E484" s="17"/>
+    </row>
+    <row r="485">
+      <c r="E485" s="17"/>
+    </row>
+    <row r="486">
+      <c r="E486" s="17"/>
+    </row>
+    <row r="487">
+      <c r="E487" s="17"/>
+    </row>
+    <row r="488">
+      <c r="E488" s="17"/>
+    </row>
+    <row r="489">
+      <c r="E489" s="17"/>
+    </row>
+    <row r="490">
+      <c r="E490" s="17"/>
+    </row>
+    <row r="491">
+      <c r="E491" s="17"/>
+    </row>
+    <row r="492">
+      <c r="E492" s="17"/>
+    </row>
+    <row r="493">
+      <c r="E493" s="17"/>
+    </row>
+    <row r="494">
+      <c r="E494" s="17"/>
+    </row>
+    <row r="495">
+      <c r="E495" s="17"/>
+    </row>
+    <row r="496">
+      <c r="E496" s="17"/>
+    </row>
+    <row r="497">
+      <c r="E497" s="17"/>
+    </row>
+    <row r="498">
+      <c r="E498" s="17"/>
+    </row>
+    <row r="499">
+      <c r="E499" s="17"/>
+    </row>
+    <row r="500">
+      <c r="E500" s="17"/>
+    </row>
+    <row r="501">
+      <c r="E501" s="17"/>
+    </row>
+    <row r="502">
+      <c r="E502" s="17"/>
+    </row>
+    <row r="503">
+      <c r="E503" s="17"/>
+    </row>
+    <row r="504">
+      <c r="E504" s="17"/>
+    </row>
+    <row r="505">
+      <c r="E505" s="17"/>
+    </row>
+    <row r="506">
+      <c r="E506" s="17"/>
+    </row>
+    <row r="507">
+      <c r="E507" s="17"/>
+    </row>
+    <row r="508">
+      <c r="E508" s="17"/>
+    </row>
+    <row r="509">
+      <c r="E509" s="17"/>
+    </row>
+    <row r="510">
+      <c r="E510" s="17"/>
+    </row>
+    <row r="511">
+      <c r="E511" s="17"/>
+    </row>
+    <row r="512">
+      <c r="E512" s="17"/>
+    </row>
+    <row r="513">
+      <c r="E513" s="17"/>
+    </row>
+    <row r="514">
+      <c r="E514" s="17"/>
+    </row>
+    <row r="515">
+      <c r="E515" s="17"/>
+    </row>
+    <row r="516">
+      <c r="E516" s="17"/>
+    </row>
+    <row r="517">
+      <c r="E517" s="17"/>
+    </row>
+    <row r="518">
+      <c r="E518" s="17"/>
+    </row>
+    <row r="519">
+      <c r="E519" s="17"/>
+    </row>
+    <row r="520">
+      <c r="E520" s="17"/>
+    </row>
+    <row r="521">
+      <c r="E521" s="17"/>
+    </row>
+    <row r="522">
+      <c r="E522" s="17"/>
+    </row>
+    <row r="523">
+      <c r="E523" s="17"/>
+    </row>
+    <row r="524">
+      <c r="E524" s="17"/>
+    </row>
+    <row r="525">
+      <c r="E525" s="17"/>
+    </row>
+    <row r="526">
+      <c r="E526" s="17"/>
+    </row>
+    <row r="527">
+      <c r="E527" s="17"/>
+    </row>
+    <row r="528">
+      <c r="E528" s="17"/>
+    </row>
+    <row r="529">
+      <c r="E529" s="17"/>
+    </row>
+    <row r="530">
+      <c r="E530" s="17"/>
+    </row>
+    <row r="531">
+      <c r="E531" s="17"/>
+    </row>
+    <row r="532">
+      <c r="E532" s="17"/>
+    </row>
+    <row r="533">
+      <c r="E533" s="17"/>
+    </row>
+    <row r="534">
+      <c r="E534" s="17"/>
+    </row>
+    <row r="535">
+      <c r="E535" s="17"/>
+    </row>
+    <row r="536">
+      <c r="E536" s="17"/>
+    </row>
+    <row r="537">
+      <c r="E537" s="17"/>
+    </row>
+    <row r="538">
+      <c r="E538" s="17"/>
+    </row>
+    <row r="539">
+      <c r="E539" s="17"/>
+    </row>
+    <row r="540">
+      <c r="E540" s="17"/>
+    </row>
+    <row r="541">
+      <c r="E541" s="17"/>
+    </row>
+    <row r="542">
+      <c r="E542" s="17"/>
+    </row>
+    <row r="543">
+      <c r="E543" s="17"/>
+    </row>
+    <row r="544">
+      <c r="E544" s="17"/>
+    </row>
+    <row r="545">
+      <c r="E545" s="17"/>
+    </row>
+    <row r="546">
+      <c r="E546" s="17"/>
+    </row>
+    <row r="547">
+      <c r="E547" s="17"/>
+    </row>
+    <row r="548">
+      <c r="E548" s="17"/>
+    </row>
+    <row r="549">
+      <c r="E549" s="17"/>
+    </row>
+    <row r="550">
+      <c r="E550" s="17"/>
+    </row>
+    <row r="551">
+      <c r="E551" s="17"/>
+    </row>
+    <row r="552">
+      <c r="E552" s="17"/>
+    </row>
+    <row r="553">
+      <c r="E553" s="17"/>
+    </row>
+    <row r="554">
+      <c r="E554" s="17"/>
+    </row>
+    <row r="555">
+      <c r="E555" s="17"/>
+    </row>
+    <row r="556">
+      <c r="E556" s="17"/>
+    </row>
+    <row r="557">
+      <c r="E557" s="17"/>
+    </row>
+    <row r="558">
+      <c r="E558" s="17"/>
+    </row>
+    <row r="559">
+      <c r="E559" s="17"/>
+    </row>
+    <row r="560">
+      <c r="E560" s="17"/>
+    </row>
+    <row r="561">
+      <c r="E561" s="17"/>
+    </row>
+    <row r="562">
+      <c r="E562" s="17"/>
+    </row>
+    <row r="563">
+      <c r="E563" s="17"/>
+    </row>
+    <row r="564">
+      <c r="E564" s="17"/>
+    </row>
+    <row r="565">
+      <c r="E565" s="17"/>
+    </row>
+    <row r="566">
+      <c r="E566" s="17"/>
+    </row>
+    <row r="567">
+      <c r="E567" s="17"/>
+    </row>
+    <row r="568">
+      <c r="E568" s="17"/>
+    </row>
+    <row r="569">
+      <c r="E569" s="17"/>
+    </row>
+    <row r="570">
+      <c r="E570" s="17"/>
+    </row>
+    <row r="571">
+      <c r="E571" s="17"/>
+    </row>
+    <row r="572">
+      <c r="E572" s="17"/>
+    </row>
+    <row r="573">
+      <c r="E573" s="17"/>
+    </row>
+    <row r="574">
+      <c r="E574" s="17"/>
+    </row>
+    <row r="575">
+      <c r="E575" s="17"/>
+    </row>
+    <row r="576">
+      <c r="E576" s="17"/>
+    </row>
+    <row r="577">
+      <c r="E577" s="17"/>
+    </row>
+    <row r="578">
+      <c r="E578" s="17"/>
+    </row>
+    <row r="579">
+      <c r="E579" s="17"/>
+    </row>
+    <row r="580">
+      <c r="E580" s="17"/>
+    </row>
+    <row r="581">
+      <c r="E581" s="17"/>
+    </row>
+    <row r="582">
+      <c r="E582" s="17"/>
+    </row>
+    <row r="583">
+      <c r="E583" s="17"/>
+    </row>
+    <row r="584">
+      <c r="E584" s="17"/>
+    </row>
+    <row r="585">
+      <c r="E585" s="17"/>
+    </row>
+    <row r="586">
+      <c r="E586" s="17"/>
+    </row>
+    <row r="587">
+      <c r="E587" s="17"/>
+    </row>
+    <row r="588">
+      <c r="E588" s="17"/>
+    </row>
+    <row r="589">
+      <c r="E589" s="17"/>
+    </row>
+    <row r="590">
+      <c r="E590" s="17"/>
+    </row>
+    <row r="591">
+      <c r="E591" s="17"/>
+    </row>
+    <row r="592">
+      <c r="E592" s="17"/>
+    </row>
+    <row r="593">
+      <c r="E593" s="17"/>
+    </row>
+    <row r="594">
+      <c r="E594" s="17"/>
+    </row>
+    <row r="595">
+      <c r="E595" s="17"/>
+    </row>
+    <row r="596">
+      <c r="E596" s="17"/>
+    </row>
+    <row r="597">
+      <c r="E597" s="17"/>
+    </row>
+    <row r="598">
+      <c r="E598" s="17"/>
+    </row>
+    <row r="599">
+      <c r="E599" s="17"/>
+    </row>
+    <row r="600">
+      <c r="E600" s="17"/>
+    </row>
+    <row r="601">
+      <c r="E601" s="17"/>
+    </row>
+    <row r="602">
+      <c r="E602" s="17"/>
+    </row>
+    <row r="603">
+      <c r="E603" s="17"/>
+    </row>
+    <row r="604">
+      <c r="E604" s="17"/>
+    </row>
+    <row r="605">
+      <c r="E605" s="17"/>
+    </row>
+    <row r="606">
+      <c r="E606" s="17"/>
+    </row>
+    <row r="607">
+      <c r="E607" s="17"/>
+    </row>
+    <row r="608">
+      <c r="E608" s="17"/>
+    </row>
+    <row r="609">
+      <c r="E609" s="17"/>
+    </row>
+    <row r="610">
+      <c r="E610" s="17"/>
+    </row>
+    <row r="611">
+      <c r="E611" s="17"/>
+    </row>
+    <row r="612">
+      <c r="E612" s="17"/>
+    </row>
+    <row r="613">
+      <c r="E613" s="17"/>
+    </row>
+    <row r="614">
+      <c r="E614" s="17"/>
+    </row>
+    <row r="615">
+      <c r="E615" s="17"/>
+    </row>
+    <row r="616">
+      <c r="E616" s="17"/>
+    </row>
+    <row r="617">
+      <c r="E617" s="17"/>
+    </row>
+    <row r="618">
+      <c r="E618" s="17"/>
+    </row>
+    <row r="619">
+      <c r="E619" s="17"/>
+    </row>
+    <row r="620">
+      <c r="E620" s="17"/>
+    </row>
+    <row r="621">
+      <c r="E621" s="17"/>
+    </row>
+    <row r="622">
+      <c r="E622" s="17"/>
+    </row>
+    <row r="623">
+      <c r="E623" s="17"/>
+    </row>
+    <row r="624">
+      <c r="E624" s="17"/>
+    </row>
+    <row r="625">
+      <c r="E625" s="17"/>
+    </row>
+    <row r="626">
+      <c r="E626" s="17"/>
+    </row>
+    <row r="627">
+      <c r="E627" s="17"/>
+    </row>
+    <row r="628">
+      <c r="E628" s="17"/>
+    </row>
+    <row r="629">
+      <c r="E629" s="17"/>
+    </row>
+    <row r="630">
+      <c r="E630" s="17"/>
+    </row>
+    <row r="631">
+      <c r="E631" s="17"/>
+    </row>
+    <row r="632">
+      <c r="E632" s="17"/>
+    </row>
+    <row r="633">
+      <c r="E633" s="17"/>
+    </row>
+    <row r="634">
+      <c r="E634" s="17"/>
+    </row>
+    <row r="635">
+      <c r="E635" s="17"/>
+    </row>
+    <row r="636">
+      <c r="E636" s="17"/>
+    </row>
+    <row r="637">
+      <c r="E637" s="17"/>
+    </row>
+    <row r="638">
+      <c r="E638" s="17"/>
+    </row>
+    <row r="639">
+      <c r="E639" s="17"/>
+    </row>
+    <row r="640">
+      <c r="E640" s="17"/>
+    </row>
+    <row r="641">
+      <c r="E641" s="17"/>
+    </row>
+    <row r="642">
+      <c r="E642" s="17"/>
+    </row>
+    <row r="643">
+      <c r="E643" s="17"/>
+    </row>
+    <row r="644">
+      <c r="E644" s="17"/>
+    </row>
+    <row r="645">
+      <c r="E645" s="17"/>
+    </row>
+    <row r="646">
+      <c r="E646" s="17"/>
+    </row>
+    <row r="647">
+      <c r="E647" s="17"/>
+    </row>
+    <row r="648">
+      <c r="E648" s="17"/>
+    </row>
+    <row r="649">
+      <c r="E649" s="17"/>
+    </row>
+    <row r="650">
+      <c r="E650" s="17"/>
+    </row>
+    <row r="651">
+      <c r="E651" s="17"/>
+    </row>
+    <row r="652">
+      <c r="E652" s="17"/>
+    </row>
+    <row r="653">
+      <c r="E653" s="17"/>
+    </row>
+    <row r="654">
+      <c r="E654" s="17"/>
+    </row>
+    <row r="655">
+      <c r="E655" s="17"/>
+    </row>
+    <row r="656">
+      <c r="E656" s="17"/>
+    </row>
+    <row r="657">
+      <c r="E657" s="17"/>
+    </row>
+    <row r="658">
+      <c r="E658" s="17"/>
+    </row>
+    <row r="659">
+      <c r="E659" s="17"/>
+    </row>
+    <row r="660">
+      <c r="E660" s="17"/>
+    </row>
+    <row r="661">
+      <c r="E661" s="17"/>
+    </row>
+    <row r="662">
+      <c r="E662" s="17"/>
+    </row>
+    <row r="663">
+      <c r="E663" s="17"/>
+    </row>
+    <row r="664">
+      <c r="E664" s="17"/>
+    </row>
+    <row r="665">
+      <c r="E665" s="17"/>
+    </row>
+    <row r="666">
+      <c r="E666" s="17"/>
+    </row>
+    <row r="667">
+      <c r="E667" s="17"/>
+    </row>
+    <row r="668">
+      <c r="E668" s="17"/>
+    </row>
+    <row r="669">
+      <c r="E669" s="17"/>
+    </row>
+    <row r="670">
+      <c r="E670" s="17"/>
+    </row>
+    <row r="671">
+      <c r="E671" s="17"/>
+    </row>
+    <row r="672">
+      <c r="E672" s="17"/>
+    </row>
+    <row r="673">
+      <c r="E673" s="17"/>
+    </row>
+    <row r="674">
+      <c r="E674" s="17"/>
+    </row>
+    <row r="675">
+      <c r="E675" s="17"/>
+    </row>
+    <row r="676">
+      <c r="E676" s="17"/>
+    </row>
+    <row r="677">
+      <c r="E677" s="17"/>
+    </row>
+    <row r="678">
+      <c r="E678" s="17"/>
+    </row>
+    <row r="679">
+      <c r="E679" s="17"/>
+    </row>
+    <row r="680">
+      <c r="E680" s="17"/>
+    </row>
+    <row r="681">
+      <c r="E681" s="17"/>
+    </row>
+    <row r="682">
+      <c r="E682" s="17"/>
+    </row>
+    <row r="683">
+      <c r="E683" s="17"/>
+    </row>
+    <row r="684">
+      <c r="E684" s="17"/>
+    </row>
+    <row r="685">
+      <c r="E685" s="17"/>
+    </row>
+    <row r="686">
+      <c r="E686" s="17"/>
+    </row>
+    <row r="687">
+      <c r="E687" s="17"/>
+    </row>
+    <row r="688">
+      <c r="E688" s="17"/>
+    </row>
+    <row r="689">
+      <c r="E689" s="17"/>
+    </row>
+    <row r="690">
+      <c r="E690" s="17"/>
+    </row>
+    <row r="691">
+      <c r="E691" s="17"/>
+    </row>
+    <row r="692">
+      <c r="E692" s="17"/>
+    </row>
+    <row r="693">
+      <c r="E693" s="17"/>
+    </row>
+    <row r="694">
+      <c r="E694" s="17"/>
+    </row>
+    <row r="695">
+      <c r="E695" s="17"/>
+    </row>
+    <row r="696">
+      <c r="E696" s="17"/>
+    </row>
+    <row r="697">
+      <c r="E697" s="17"/>
+    </row>
+    <row r="698">
+      <c r="E698" s="17"/>
+    </row>
+    <row r="699">
+      <c r="E699" s="17"/>
+    </row>
+    <row r="700">
+      <c r="E700" s="17"/>
+    </row>
+    <row r="701">
+      <c r="E701" s="17"/>
+    </row>
+    <row r="702">
+      <c r="E702" s="17"/>
+    </row>
+    <row r="703">
+      <c r="E703" s="17"/>
+    </row>
+    <row r="704">
+      <c r="E704" s="17"/>
+    </row>
+    <row r="705">
+      <c r="E705" s="17"/>
+    </row>
+    <row r="706">
+      <c r="E706" s="17"/>
+    </row>
+    <row r="707">
+      <c r="E707" s="17"/>
+    </row>
+    <row r="708">
+      <c r="E708" s="17"/>
+    </row>
+    <row r="709">
+      <c r="E709" s="17"/>
+    </row>
+    <row r="710">
+      <c r="E710" s="17"/>
+    </row>
+    <row r="711">
+      <c r="E711" s="17"/>
+    </row>
+    <row r="712">
+      <c r="E712" s="17"/>
+    </row>
+    <row r="713">
+      <c r="E713" s="17"/>
+    </row>
+    <row r="714">
+      <c r="E714" s="17"/>
+    </row>
+    <row r="715">
+      <c r="E715" s="17"/>
+    </row>
+    <row r="716">
+      <c r="E716" s="17"/>
+    </row>
+    <row r="717">
+      <c r="E717" s="17"/>
+    </row>
+    <row r="718">
+      <c r="E718" s="17"/>
+    </row>
+    <row r="719">
+      <c r="E719" s="17"/>
+    </row>
+    <row r="720">
+      <c r="E720" s="17"/>
+    </row>
+    <row r="721">
+      <c r="E721" s="17"/>
+    </row>
+    <row r="722">
+      <c r="E722" s="17"/>
+    </row>
+    <row r="723">
+      <c r="E723" s="17"/>
+    </row>
+    <row r="724">
+      <c r="E724" s="17"/>
+    </row>
+    <row r="725">
+      <c r="E725" s="17"/>
+    </row>
+    <row r="726">
+      <c r="E726" s="17"/>
+    </row>
+    <row r="727">
+      <c r="E727" s="17"/>
+    </row>
+    <row r="728">
+      <c r="E728" s="17"/>
+    </row>
+    <row r="729">
+      <c r="E729" s="17"/>
+    </row>
+    <row r="730">
+      <c r="E730" s="17"/>
+    </row>
+    <row r="731">
+      <c r="E731" s="17"/>
+    </row>
+    <row r="732">
+      <c r="E732" s="17"/>
+    </row>
+    <row r="733">
+      <c r="E733" s="17"/>
+    </row>
+    <row r="734">
+      <c r="E734" s="17"/>
+    </row>
+    <row r="735">
+      <c r="E735" s="17"/>
+    </row>
+    <row r="736">
+      <c r="E736" s="17"/>
+    </row>
+    <row r="737">
+      <c r="E737" s="17"/>
+    </row>
+    <row r="738">
+      <c r="E738" s="17"/>
+    </row>
+    <row r="739">
+      <c r="E739" s="17"/>
+    </row>
+    <row r="740">
+      <c r="E740" s="17"/>
+    </row>
+    <row r="741">
+      <c r="E741" s="17"/>
+    </row>
+    <row r="742">
+      <c r="E742" s="17"/>
+    </row>
+    <row r="743">
+      <c r="E743" s="17"/>
+    </row>
+    <row r="744">
+      <c r="E744" s="17"/>
+    </row>
+    <row r="745">
+      <c r="E745" s="17"/>
+    </row>
+    <row r="746">
+      <c r="E746" s="17"/>
+    </row>
+    <row r="747">
+      <c r="E747" s="17"/>
+    </row>
+    <row r="748">
+      <c r="E748" s="17"/>
+    </row>
+    <row r="749">
+      <c r="E749" s="17"/>
+    </row>
+    <row r="750">
+      <c r="E750" s="17"/>
+    </row>
+    <row r="751">
+      <c r="E751" s="17"/>
+    </row>
+    <row r="752">
+      <c r="E752" s="17"/>
+    </row>
+    <row r="753">
+      <c r="E753" s="17"/>
+    </row>
+    <row r="754">
+      <c r="E754" s="17"/>
+    </row>
+    <row r="755">
+      <c r="E755" s="17"/>
+    </row>
+    <row r="756">
+      <c r="E756" s="17"/>
+    </row>
+    <row r="757">
+      <c r="E757" s="17"/>
+    </row>
+    <row r="758">
+      <c r="E758" s="17"/>
+    </row>
+    <row r="759">
+      <c r="E759" s="17"/>
+    </row>
+    <row r="760">
+      <c r="E760" s="17"/>
+    </row>
+    <row r="761">
+      <c r="E761" s="17"/>
+    </row>
+    <row r="762">
+      <c r="E762" s="17"/>
+    </row>
+    <row r="763">
+      <c r="E763" s="17"/>
+    </row>
+    <row r="764">
+      <c r="E764" s="17"/>
+    </row>
+    <row r="765">
+      <c r="E765" s="17"/>
+    </row>
+    <row r="766">
+      <c r="E766" s="17"/>
+    </row>
+    <row r="767">
+      <c r="E767" s="17"/>
+    </row>
+    <row r="768">
+      <c r="E768" s="17"/>
+    </row>
+    <row r="769">
+      <c r="E769" s="17"/>
+    </row>
+    <row r="770">
+      <c r="E770" s="17"/>
+    </row>
+    <row r="771">
+      <c r="E771" s="17"/>
+    </row>
+    <row r="772">
+      <c r="E772" s="17"/>
+    </row>
+    <row r="773">
+      <c r="E773" s="17"/>
+    </row>
+    <row r="774">
+      <c r="E774" s="17"/>
+    </row>
+    <row r="775">
+      <c r="E775" s="17"/>
+    </row>
+    <row r="776">
+      <c r="E776" s="17"/>
+    </row>
+    <row r="777">
+      <c r="E777" s="17"/>
+    </row>
+    <row r="778">
+      <c r="E778" s="17"/>
+    </row>
+    <row r="779">
+      <c r="E779" s="17"/>
+    </row>
+    <row r="780">
+      <c r="E780" s="17"/>
+    </row>
+    <row r="781">
+      <c r="E781" s="17"/>
+    </row>
+    <row r="782">
+      <c r="E782" s="17"/>
+    </row>
+    <row r="783">
+      <c r="E783" s="17"/>
+    </row>
+    <row r="784">
+      <c r="E784" s="17"/>
+    </row>
+    <row r="785">
+      <c r="E785" s="17"/>
+    </row>
+    <row r="786">
+      <c r="E786" s="17"/>
+    </row>
+    <row r="787">
+      <c r="E787" s="17"/>
+    </row>
+    <row r="788">
+      <c r="E788" s="17"/>
+    </row>
+    <row r="789">
+      <c r="E789" s="17"/>
+    </row>
+    <row r="790">
+      <c r="E790" s="17"/>
+    </row>
+    <row r="791">
+      <c r="E791" s="17"/>
+    </row>
+    <row r="792">
+      <c r="E792" s="17"/>
+    </row>
+    <row r="793">
+      <c r="E793" s="17"/>
+    </row>
+    <row r="794">
+      <c r="E794" s="17"/>
+    </row>
+    <row r="795">
+      <c r="E795" s="17"/>
+    </row>
+    <row r="796">
+      <c r="E796" s="17"/>
+    </row>
+    <row r="797">
+      <c r="E797" s="17"/>
+    </row>
+    <row r="798">
+      <c r="E798" s="17"/>
+    </row>
+    <row r="799">
+      <c r="E799" s="17"/>
+    </row>
+    <row r="800">
+      <c r="E800" s="17"/>
+    </row>
+    <row r="801">
+      <c r="E801" s="17"/>
+    </row>
+    <row r="802">
+      <c r="E802" s="17"/>
+    </row>
+    <row r="803">
+      <c r="E803" s="17"/>
+    </row>
+    <row r="804">
+      <c r="E804" s="17"/>
+    </row>
+    <row r="805">
+      <c r="E805" s="17"/>
+    </row>
+    <row r="806">
+      <c r="E806" s="17"/>
+    </row>
+    <row r="807">
+      <c r="E807" s="17"/>
+    </row>
+    <row r="808">
+      <c r="E808" s="17"/>
+    </row>
+    <row r="809">
+      <c r="E809" s="17"/>
+    </row>
+    <row r="810">
+      <c r="E810" s="17"/>
+    </row>
+    <row r="811">
+      <c r="E811" s="17"/>
+    </row>
+    <row r="812">
+      <c r="E812" s="17"/>
+    </row>
+    <row r="813">
+      <c r="E813" s="17"/>
+    </row>
+    <row r="814">
+      <c r="E814" s="17"/>
+    </row>
+    <row r="815">
+      <c r="E815" s="17"/>
+    </row>
+    <row r="816">
+      <c r="E816" s="17"/>
+    </row>
+    <row r="817">
+      <c r="E817" s="17"/>
+    </row>
+    <row r="818">
+      <c r="E818" s="17"/>
+    </row>
+    <row r="819">
+      <c r="E819" s="17"/>
+    </row>
+    <row r="820">
+      <c r="E820" s="17"/>
+    </row>
+    <row r="821">
+      <c r="E821" s="17"/>
+    </row>
+    <row r="822">
+      <c r="E822" s="17"/>
+    </row>
+    <row r="823">
+      <c r="E823" s="17"/>
+    </row>
+    <row r="824">
+      <c r="E824" s="17"/>
+    </row>
+    <row r="825">
+      <c r="E825" s="17"/>
+    </row>
+    <row r="826">
+      <c r="E826" s="17"/>
+    </row>
+    <row r="827">
+      <c r="E827" s="17"/>
+    </row>
+    <row r="828">
+      <c r="E828" s="17"/>
+    </row>
+    <row r="829">
+      <c r="E829" s="17"/>
+    </row>
+    <row r="830">
+      <c r="E830" s="17"/>
+    </row>
+    <row r="831">
+      <c r="E831" s="17"/>
+    </row>
+    <row r="832">
+      <c r="E832" s="17"/>
+    </row>
+    <row r="833">
+      <c r="E833" s="17"/>
+    </row>
+    <row r="834">
+      <c r="E834" s="17"/>
+    </row>
+    <row r="835">
+      <c r="E835" s="17"/>
+    </row>
+    <row r="836">
+      <c r="E836" s="17"/>
+    </row>
+    <row r="837">
+      <c r="E837" s="17"/>
+    </row>
+    <row r="838">
+      <c r="E838" s="17"/>
+    </row>
+    <row r="839">
+      <c r="E839" s="17"/>
+    </row>
+    <row r="840">
+      <c r="E840" s="17"/>
+    </row>
+    <row r="841">
+      <c r="E841" s="17"/>
+    </row>
+    <row r="842">
+      <c r="E842" s="17"/>
+    </row>
+    <row r="843">
+      <c r="E843" s="17"/>
+    </row>
+    <row r="844">
+      <c r="E844" s="17"/>
+    </row>
+    <row r="845">
+      <c r="E845" s="17"/>
+    </row>
+    <row r="846">
+      <c r="E846" s="17"/>
+    </row>
+    <row r="847">
+      <c r="E847" s="17"/>
+    </row>
+    <row r="848">
+      <c r="E848" s="17"/>
+    </row>
+    <row r="849">
+      <c r="E849" s="17"/>
+    </row>
+    <row r="850">
+      <c r="E850" s="17"/>
+    </row>
+    <row r="851">
+      <c r="E851" s="17"/>
+    </row>
+    <row r="852">
+      <c r="E852" s="17"/>
+    </row>
+    <row r="853">
+      <c r="E853" s="17"/>
+    </row>
+    <row r="854">
+      <c r="E854" s="17"/>
+    </row>
+    <row r="855">
+      <c r="E855" s="17"/>
+    </row>
+    <row r="856">
+      <c r="E856" s="17"/>
+    </row>
+    <row r="857">
+      <c r="E857" s="17"/>
+    </row>
+    <row r="858">
+      <c r="E858" s="17"/>
+    </row>
+    <row r="859">
+      <c r="E859" s="17"/>
+    </row>
+    <row r="860">
+      <c r="E860" s="17"/>
+    </row>
+    <row r="861">
+      <c r="E861" s="17"/>
+    </row>
+    <row r="862">
+      <c r="E862" s="17"/>
+    </row>
+    <row r="863">
+      <c r="E863" s="17"/>
+    </row>
+    <row r="864">
+      <c r="E864" s="17"/>
+    </row>
+    <row r="865">
+      <c r="E865" s="17"/>
+    </row>
+    <row r="866">
+      <c r="E866" s="17"/>
+    </row>
+    <row r="867">
+      <c r="E867" s="17"/>
+    </row>
+    <row r="868">
+      <c r="E868" s="17"/>
+    </row>
+    <row r="869">
+      <c r="E869" s="17"/>
+    </row>
+    <row r="870">
+      <c r="E870" s="17"/>
+    </row>
+    <row r="871">
+      <c r="E871" s="17"/>
+    </row>
+    <row r="872">
+      <c r="E872" s="17"/>
+    </row>
+    <row r="873">
+      <c r="E873" s="17"/>
+    </row>
+    <row r="874">
+      <c r="E874" s="17"/>
+    </row>
+    <row r="875">
+      <c r="E875" s="17"/>
+    </row>
+    <row r="876">
+      <c r="E876" s="17"/>
+    </row>
+    <row r="877">
+      <c r="E877" s="17"/>
+    </row>
+    <row r="878">
+      <c r="E878" s="17"/>
+    </row>
+    <row r="879">
+      <c r="E879" s="17"/>
+    </row>
+    <row r="880">
+      <c r="E880" s="17"/>
+    </row>
+    <row r="881">
+      <c r="E881" s="17"/>
+    </row>
+    <row r="882">
+      <c r="E882" s="17"/>
+    </row>
+    <row r="883">
+      <c r="E883" s="17"/>
+    </row>
+    <row r="884">
+      <c r="E884" s="17"/>
+    </row>
+    <row r="885">
+      <c r="E885" s="17"/>
+    </row>
+    <row r="886">
+      <c r="E886" s="17"/>
+    </row>
+    <row r="887">
+      <c r="E887" s="17"/>
+    </row>
+    <row r="888">
+      <c r="E888" s="17"/>
+    </row>
+    <row r="889">
+      <c r="E889" s="17"/>
+    </row>
+    <row r="890">
+      <c r="E890" s="17"/>
+    </row>
+    <row r="891">
+      <c r="E891" s="17"/>
+    </row>
+    <row r="892">
+      <c r="E892" s="17"/>
+    </row>
+    <row r="893">
+      <c r="E893" s="17"/>
+    </row>
+    <row r="894">
+      <c r="E894" s="17"/>
+    </row>
+    <row r="895">
+      <c r="E895" s="17"/>
+    </row>
+    <row r="896">
+      <c r="E896" s="17"/>
+    </row>
+    <row r="897">
+      <c r="E897" s="17"/>
+    </row>
+    <row r="898">
+      <c r="E898" s="17"/>
+    </row>
+    <row r="899">
+      <c r="E899" s="17"/>
+    </row>
+    <row r="900">
+      <c r="E900" s="17"/>
+    </row>
+    <row r="901">
+      <c r="E901" s="17"/>
+    </row>
+    <row r="902">
+      <c r="E902" s="17"/>
+    </row>
+    <row r="903">
+      <c r="E903" s="17"/>
+    </row>
+    <row r="904">
+      <c r="E904" s="17"/>
+    </row>
+    <row r="905">
+      <c r="E905" s="17"/>
+    </row>
+    <row r="906">
+      <c r="E906" s="17"/>
+    </row>
+    <row r="907">
+      <c r="E907" s="17"/>
+    </row>
+    <row r="908">
+      <c r="E908" s="17"/>
+    </row>
+    <row r="909">
+      <c r="E909" s="17"/>
+    </row>
+    <row r="910">
+      <c r="E910" s="17"/>
+    </row>
+    <row r="911">
+      <c r="E911" s="17"/>
+    </row>
+    <row r="912">
+      <c r="E912" s="17"/>
+    </row>
+    <row r="913">
+      <c r="E913" s="17"/>
+    </row>
+    <row r="914">
+      <c r="E914" s="17"/>
+    </row>
+    <row r="915">
+      <c r="E915" s="17"/>
+    </row>
+    <row r="916">
+      <c r="E916" s="17"/>
+    </row>
+    <row r="917">
+      <c r="E917" s="17"/>
+    </row>
+    <row r="918">
+      <c r="E918" s="17"/>
+    </row>
+    <row r="919">
+      <c r="E919" s="17"/>
+    </row>
+    <row r="920">
+      <c r="E920" s="17"/>
+    </row>
+    <row r="921">
+      <c r="E921" s="17"/>
+    </row>
+    <row r="922">
+      <c r="E922" s="17"/>
+    </row>
+    <row r="923">
+      <c r="E923" s="17"/>
+    </row>
+    <row r="924">
+      <c r="E924" s="17"/>
+    </row>
+    <row r="925">
+      <c r="E925" s="17"/>
+    </row>
+    <row r="926">
+      <c r="E926" s="17"/>
+    </row>
+    <row r="927">
+      <c r="E927" s="17"/>
+    </row>
+    <row r="928">
+      <c r="E928" s="17"/>
+    </row>
+    <row r="929">
+      <c r="E929" s="17"/>
+    </row>
+    <row r="930">
+      <c r="E930" s="17"/>
+    </row>
+    <row r="931">
+      <c r="E931" s="17"/>
+    </row>
+    <row r="932">
+      <c r="E932" s="17"/>
+    </row>
+    <row r="933">
+      <c r="E933" s="17"/>
+    </row>
+    <row r="934">
+      <c r="E934" s="17"/>
+    </row>
+    <row r="935">
+      <c r="E935" s="17"/>
+    </row>
+    <row r="936">
+      <c r="E936" s="17"/>
+    </row>
+    <row r="937">
+      <c r="E937" s="17"/>
+    </row>
+    <row r="938">
+      <c r="E938" s="17"/>
+    </row>
+    <row r="939">
+      <c r="E939" s="17"/>
+    </row>
+    <row r="940">
+      <c r="E940" s="17"/>
+    </row>
+    <row r="941">
+      <c r="E941" s="17"/>
+    </row>
+    <row r="942">
+      <c r="E942" s="17"/>
+    </row>
+    <row r="943">
+      <c r="E943" s="17"/>
+    </row>
+    <row r="944">
+      <c r="E944" s="17"/>
+    </row>
+    <row r="945">
+      <c r="E945" s="17"/>
+    </row>
+    <row r="946">
+      <c r="E946" s="17"/>
+    </row>
+    <row r="947">
+      <c r="E947" s="17"/>
+    </row>
+    <row r="948">
+      <c r="E948" s="17"/>
+    </row>
+    <row r="949">
+      <c r="E949" s="17"/>
+    </row>
+    <row r="950">
+      <c r="E950" s="17"/>
+    </row>
+    <row r="951">
+      <c r="E951" s="17"/>
+    </row>
+    <row r="952">
+      <c r="E952" s="17"/>
+    </row>
+    <row r="953">
+      <c r="E953" s="17"/>
+    </row>
+    <row r="954">
+      <c r="E954" s="17"/>
+    </row>
+    <row r="955">
+      <c r="E955" s="17"/>
+    </row>
+    <row r="956">
+      <c r="E956" s="17"/>
+    </row>
+    <row r="957">
+      <c r="E957" s="17"/>
+    </row>
+    <row r="958">
+      <c r="E958" s="17"/>
+    </row>
+    <row r="959">
+      <c r="E959" s="17"/>
+    </row>
+    <row r="960">
+      <c r="E960" s="17"/>
+    </row>
+    <row r="961">
+      <c r="E961" s="17"/>
+    </row>
+    <row r="962">
+      <c r="E962" s="17"/>
+    </row>
+    <row r="963">
+      <c r="E963" s="17"/>
+    </row>
+    <row r="964">
+      <c r="E964" s="17"/>
+    </row>
+    <row r="965">
+      <c r="E965" s="17"/>
+    </row>
+    <row r="966">
+      <c r="E966" s="17"/>
+    </row>
+    <row r="967">
+      <c r="E967" s="17"/>
+    </row>
+    <row r="968">
+      <c r="E968" s="17"/>
+    </row>
+    <row r="969">
+      <c r="E969" s="17"/>
+    </row>
+    <row r="970">
+      <c r="E970" s="17"/>
+    </row>
+    <row r="971">
+      <c r="E971" s="17"/>
+    </row>
+    <row r="972">
+      <c r="E972" s="17"/>
+    </row>
+    <row r="973">
+      <c r="E973" s="17"/>
+    </row>
+    <row r="974">
+      <c r="E974" s="17"/>
+    </row>
+    <row r="975">
+      <c r="E975" s="17"/>
+    </row>
+    <row r="976">
+      <c r="E976" s="17"/>
+    </row>
+    <row r="977">
+      <c r="E977" s="17"/>
+    </row>
+    <row r="978">
+      <c r="E978" s="17"/>
+    </row>
+    <row r="979">
+      <c r="E979" s="17"/>
+    </row>
+    <row r="980">
+      <c r="E980" s="17"/>
+    </row>
+    <row r="981">
+      <c r="E981" s="17"/>
+    </row>
+    <row r="982">
+      <c r="E982" s="17"/>
+    </row>
+    <row r="983">
+      <c r="E983" s="17"/>
+    </row>
+    <row r="984">
+      <c r="E984" s="17"/>
+    </row>
+    <row r="985">
+      <c r="E985" s="17"/>
+    </row>
+    <row r="986">
+      <c r="E986" s="17"/>
+    </row>
+    <row r="987">
+      <c r="E987" s="17"/>
+    </row>
+    <row r="988">
+      <c r="E988" s="17"/>
+    </row>
+    <row r="989">
+      <c r="E989" s="17"/>
+    </row>
+    <row r="990">
+      <c r="E990" s="17"/>
+    </row>
+    <row r="991">
+      <c r="E991" s="17"/>
+    </row>
+    <row r="992">
+      <c r="E992" s="17"/>
+    </row>
+    <row r="993">
+      <c r="E993" s="17"/>
+    </row>
+    <row r="994">
+      <c r="E994" s="17"/>
+    </row>
+    <row r="995">
+      <c r="E995" s="17"/>
+    </row>
+    <row r="996">
+      <c r="E996" s="17"/>
+    </row>
+    <row r="997">
+      <c r="E997" s="17"/>
+    </row>
+    <row r="998">
+      <c r="E998" s="17"/>
+    </row>
+    <row r="999">
+      <c r="E999" s="17"/>
+    </row>
+    <row r="1000">
+      <c r="E1000" s="17"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>